<commit_message>
save results from robot_planner1 RRTConnect experiment
</commit_message>
<xml_diff>
--- a/data/Thesis Experiments.xlsx
+++ b/data/Thesis Experiments.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="robot_planner1" sheetId="1" state="visible" r:id="rId2"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="41">
   <si>
     <t xml:space="preserve">Robot Planner 1</t>
   </si>
@@ -37,6 +37,44 @@
     <t xml:space="preserve">RRTConnect</t>
   </si>
   <si>
+    <t xml:space="preserve">Experiment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Approach time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Execution 
+Status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Move away time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insertion 
+Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pivot 
+Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reverse 
+Pivot time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reverse insertion 
+Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Robot Planner 2</t>
+  </si>
+  <si>
     <t xml:space="preserve">RRT*</t>
   </si>
   <si>
@@ -44,9 +82,6 @@
   </si>
   <si>
     <t xml:space="preserve">PRM*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Experiment</t>
   </si>
   <si>
     <t xml:space="preserve">Status</t>
@@ -57,12 +92,6 @@
   <si>
     <t xml:space="preserve">Planning 
 Attempts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Average</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Robot Planner 2</t>
   </si>
   <si>
     <t xml:space="preserve">Robot Planner 3b</t>
@@ -142,7 +171,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="#,##0.000000"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -184,11 +213,6 @@
       <name val="Cambria"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Cambria"/>
-      <family val="0"/>
     </font>
     <font>
       <b val="true"/>
@@ -274,7 +298,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -290,7 +314,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -309,7 +333,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -317,7 +341,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -393,7 +417,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -423,6 +447,8 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -474,17 +500,17 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="9799505"/>
-        <c:axId val="32041794"/>
+        <c:axId val="36504027"/>
+        <c:axId val="34443877"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="9799505"/>
+        <c:axId val="36504027"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -506,12 +532,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="32041794"/>
+        <c:crossAx val="34443877"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="32041794"/>
+        <c:axId val="34443877"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -526,7 +552,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -548,7 +574,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="9799505"/>
+        <c:crossAx val="36504027"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -607,9 +633,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>99360</xdr:colOff>
+      <xdr:colOff>99000</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>154080</xdr:rowOff>
+      <xdr:rowOff>153720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -618,7 +644,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="10197000" y="9605520"/>
-        <a:ext cx="5757480" cy="3237120"/>
+        <a:ext cx="5757120" cy="3236760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -636,24 +662,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:M34"/>
+  <dimension ref="A2:O34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M22" activeCellId="0" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="8" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="4.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="17.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="14.43"/>
   </cols>
   <sheetData>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -662,96 +693,524 @@
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="E2" s="2"/>
+      <c r="G2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
-      <c r="K2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L2" s="2"/>
+      <c r="L2" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="E3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="H3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="J3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="L3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>7</v>
-      </c>
       <c r="M3" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>4</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="0" t="n">
+        <v>0.060402</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>0.144881</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>0.216565</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>3.639193</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>2.419514</v>
+      </c>
+      <c r="M4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N4" s="0" t="n">
+        <v>2.388166</v>
+      </c>
+      <c r="O4" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="n">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="0" t="n">
+        <v>0.06053</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>0.058341</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>0.057143</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>0.057187</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <v>1.386188</v>
+      </c>
+      <c r="M5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N5" s="0" t="n">
+        <v>2.874223</v>
+      </c>
+      <c r="O5" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0" t="n">
+        <v>0.064706</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>0.060981</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>0.073242</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>0.072451</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="M6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" s="0" t="n">
+        <v>5.106926</v>
+      </c>
+      <c r="O6" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="n">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0" t="n">
+        <v>0.059789</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>0.119351</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>0.056255</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>0.068156</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <v>5.466561</v>
+      </c>
+      <c r="M7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N7" s="0" t="n">
+        <v>4.562506</v>
+      </c>
+      <c r="O7" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="n">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
+      <c r="B8" s="0" t="n">
+        <v>0.164789</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>0.330373</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>0.16178</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>0.150123</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L8" s="0" t="n">
+        <v>5.62329</v>
+      </c>
+      <c r="M8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N8" s="0" t="n">
+        <v>5.587679</v>
+      </c>
+      <c r="O8" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>0.147037</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>0.289805</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>0.071426</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>0.065059</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L9" s="0" t="n">
+        <v>5.488728</v>
+      </c>
+      <c r="M9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="O9" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>0.18233</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>0.093362</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>0.155125</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="M10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="O10" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>0.054469</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>0.062209</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>0.315921</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>0.194663</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L11" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="M11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N11" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="O11" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5" t="n">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="B12" s="0" t="n">
+        <v>0.05313</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>0.409191</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>0.127381</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>0.19026</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L12" s="0" t="n">
+        <v>5.291442</v>
+      </c>
+      <c r="M12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N12" s="0" t="n">
+        <v>5.096234</v>
+      </c>
+      <c r="O12" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>0.105909</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>0.307963</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <v>0.396182</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I13" s="0" t="n">
+        <v>0.075866</v>
+      </c>
+      <c r="J13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L13" s="0" t="n">
+        <v>5.381595</v>
+      </c>
+      <c r="M13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N13" s="0" t="n">
+        <v>5.576362</v>
+      </c>
+      <c r="O13" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <f aca="false">AVERAGE(B4:B13)</f>
+        <v>0.0953091</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <f aca="false">AVERAGE(C4:C13)</f>
+        <v>1</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <f aca="false">AVERAGE(D4:D13)</f>
+        <v>0.1876457</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <f aca="false">AVERAGE(E4:E13)</f>
+        <v>1</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <f aca="false">AVERAGE(G4:G13)</f>
+        <v>0.163102</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <f aca="false">AVERAGE(H4:H13)</f>
+        <v>1</v>
+      </c>
+      <c r="I14" s="0" t="n">
+        <f aca="false">AVERAGE(I4:I13)</f>
+        <v>0.501439777777778</v>
+      </c>
+      <c r="J14" s="0" t="n">
+        <f aca="false">AVERAGE(J4:J13)</f>
+        <v>0.9</v>
+      </c>
+      <c r="L14" s="0" t="n">
+        <f aca="false">AVERAGE(L4:L13)</f>
+        <v>4.43675971428571</v>
+      </c>
+      <c r="M14" s="0" t="n">
+        <f aca="false">AVERAGE(M4:M13)</f>
+        <v>0.6</v>
+      </c>
+      <c r="N14" s="0" t="n">
+        <f aca="false">AVERAGE(N4:N13)</f>
+        <v>4.45601371428571</v>
+      </c>
+      <c r="O14" s="0" t="n">
+        <f aca="false">AVERAGE(O4:O13)</f>
+        <v>0.6</v>
+      </c>
+    </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -775,11 +1234,10 @@
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="K2:M2"/>
+  <mergeCells count="3">
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="L2:O2"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -798,8 +1256,8 @@
   </sheetPr>
   <dimension ref="A1:T40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M36" activeCellId="0" sqref="M36"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AA25" activeCellId="0" sqref="AA25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -810,53 +1268,53 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="L1" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="L1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
       <c r="G2" s="9" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H2" s="9"/>
       <c r="I2" s="9"/>
       <c r="J2" s="9"/>
       <c r="L2" s="9" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="M2" s="9"/>
       <c r="N2" s="9"/>
       <c r="O2" s="9"/>
       <c r="Q2" s="9" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="R2" s="9"/>
       <c r="S2" s="9"/>
@@ -864,55 +1322,55 @@
     </row>
     <row r="3" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="H3" s="4" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="I3" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="M3" s="8" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="N3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="O3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="R3" s="8" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="T3" s="8" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -923,7 +1381,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="D4" s="12" t="n">
         <v>0.065173</v>
@@ -1368,7 +1826,7 @@
         <v>1</v>
       </c>
       <c r="K12" s="0" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="L12" s="0" t="n">
         <v>1</v>
@@ -1433,7 +1891,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>1</v>
@@ -1469,60 +1927,60 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D17" s="0" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="N17" s="0" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D18" s="0" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="N18" s="0" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D19" s="0" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D20" s="0" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="N20" s="0" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D21" s="0" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="6"/>
+      <c r="B29" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="9" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>
       <c r="E30" s="9"/>
       <c r="G30" s="9" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H30" s="9"/>
       <c r="I30" s="9"/>
@@ -1530,34 +1988,34 @@
     </row>
     <row r="31" customFormat="false" ht="52.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="7" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D31" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G31" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E31" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="H31" s="8" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="J31" s="8" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="N31" s="13" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1589,7 +2047,7 @@
         <v>1</v>
       </c>
       <c r="N32" s="0" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1650,7 +2108,7 @@
         <v>1</v>
       </c>
       <c r="N34" s="0" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1682,7 +2140,7 @@
         <v>1</v>
       </c>
       <c r="N35" s="0" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1714,7 +2172,7 @@
         <v>1</v>
       </c>
       <c r="N36" s="0" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1777,7 +2235,7 @@
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="10" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>1</v>
@@ -1855,68 +2313,68 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="F1" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="J1" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="N1" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
+        <v>12</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="F1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="J1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="N1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="P2" s="8" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1946,7 +2404,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1985,68 +2443,68 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="F1" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="J1" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="N1" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
+        <v>19</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="F1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="J1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="N1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="P2" s="8" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2076,7 +2534,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -2115,68 +2573,68 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="F1" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="J1" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="N1" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
+        <v>19</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="F1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="J1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="N1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="P2" s="8" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2206,7 +2664,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data results for robot_planner1 rrt* experiment
</commit_message>
<xml_diff>
--- a/data/Thesis Experiments.xlsx
+++ b/data/Thesis Experiments.xlsx
@@ -29,12 +29,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="44">
   <si>
     <t xml:space="preserve">Robot Planner 1</t>
   </si>
   <si>
-    <t xml:space="preserve">RRTConnect</t>
+    <t xml:space="preserve">RRTConnect (max 5 seconds planning time)</t>
   </si>
   <si>
     <t xml:space="preserve">Experiment</t>
@@ -72,7 +72,16 @@
     <t xml:space="preserve">Average</t>
   </si>
   <si>
+    <t xml:space="preserve">RRT* (max 5 seconds planning time)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
     <t xml:space="preserve">Robot Planner 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RRTConnect</t>
   </si>
   <si>
     <t xml:space="preserve">RRT*</t>
@@ -417,7 +426,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -500,11 +509,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="36504027"/>
-        <c:axId val="34443877"/>
+        <c:axId val="32819758"/>
+        <c:axId val="11885394"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="36504027"/>
+        <c:axId val="32819758"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -532,12 +541,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="34443877"/>
+        <c:crossAx val="11885394"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="34443877"/>
+        <c:axId val="11885394"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -574,7 +583,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="36504027"/>
+        <c:crossAx val="32819758"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -633,9 +642,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>99000</xdr:colOff>
+      <xdr:colOff>98640</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>153720</xdr:rowOff>
+      <xdr:rowOff>153360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -644,7 +653,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="10197000" y="9605520"/>
-        <a:ext cx="5757120" cy="3236760"/>
+        <a:ext cx="5756760" cy="3236400"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -662,10 +671,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:O34"/>
+  <dimension ref="A2:Q34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M22" activeCellId="0" sqref="M22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M39" activeCellId="0" sqref="M39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -694,15 +703,13 @@
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="G2" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
-      <c r="L2" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
@@ -1213,17 +1220,534 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+    </row>
+    <row r="18" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M18" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="N18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="O18" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>5.096772</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>5.023175</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G19" s="0" t="n">
+        <v>5.200983</v>
+      </c>
+      <c r="H19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I19" s="0" t="n">
+        <v>5.044568</v>
+      </c>
+      <c r="J19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L19" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="M19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N19" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="O19" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>5.015857</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>5.034447</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>5.009846</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I20" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="J20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L20" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="M20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N20" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="O20" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>5.01843</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>5.101766</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>5.064216</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I21" s="0" t="n">
+        <v>5.085314</v>
+      </c>
+      <c r="J21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L21" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="M21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N21" s="0" t="n">
+        <v>5.508861</v>
+      </c>
+      <c r="O21" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>5.074703</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>5.089464</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G22" s="0" t="n">
+        <v>5.145115</v>
+      </c>
+      <c r="H22" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I22" s="0" t="n">
+        <v>5.059245</v>
+      </c>
+      <c r="J22" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L22" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="M22" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N22" s="0" t="n">
+        <v>5.417935</v>
+      </c>
+      <c r="O22" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>5.019108</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>5.056875</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G23" s="0" t="n">
+        <v>5.019322</v>
+      </c>
+      <c r="H23" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I23" s="0" t="n">
+        <v>5.173925</v>
+      </c>
+      <c r="J23" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L23" s="0" t="n">
+        <v>5.057058</v>
+      </c>
+      <c r="M23" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N23" s="0" t="n">
+        <v>5.093558</v>
+      </c>
+      <c r="O23" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>5.011631</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>5.217069</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G24" s="0" t="n">
+        <v>5.015804</v>
+      </c>
+      <c r="H24" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I24" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="J24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L24" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="M24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N24" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="O24" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>5.119638</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>5.027692</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G25" s="0" t="n">
+        <v>5.033637</v>
+      </c>
+      <c r="H25" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I25" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="J25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L25" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="M25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N25" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="O25" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>5.121159</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>5.040244</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G26" s="0" t="n">
+        <v>5.159212</v>
+      </c>
+      <c r="H26" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I26" s="0" t="n">
+        <v>5.100395</v>
+      </c>
+      <c r="J26" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L26" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="M26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N26" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="O26" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>5.12812</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>5.098381</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G27" s="0" t="n">
+        <v>5.134356</v>
+      </c>
+      <c r="H27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I27" s="0" t="n">
+        <v>5.081432</v>
+      </c>
+      <c r="J27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L27" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="M27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N27" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="O27" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>5.343964</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>5.374314</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G28" s="0" t="n">
+        <v>5.052</v>
+      </c>
+      <c r="H28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I28" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="J28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L28" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="M28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N28" s="0" t="n">
+        <v>5.358954</v>
+      </c>
+      <c r="O28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <f aca="false">AVERAGE(B19:B28)</f>
+        <v>5.0949382</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <f aca="false">AVERAGE(C19:C28)</f>
+        <v>1</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <f aca="false">AVERAGE(D19:D28)</f>
+        <v>5.1063427</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <f aca="false">AVERAGE(E19:E28)</f>
+        <v>1</v>
+      </c>
+      <c r="G29" s="0" t="n">
+        <f aca="false">AVERAGE(G19:G28)</f>
+        <v>5.0834491</v>
+      </c>
+      <c r="H29" s="0" t="n">
+        <f aca="false">AVERAGE(H19:H28)</f>
+        <v>0.9</v>
+      </c>
+      <c r="I29" s="0" t="n">
+        <f aca="false">AVERAGE(I19:I28)</f>
+        <v>5.09081316666667</v>
+      </c>
+      <c r="J29" s="0" t="n">
+        <f aca="false">AVERAGE(J19:J28)</f>
+        <v>0.6</v>
+      </c>
+      <c r="L29" s="0" t="n">
+        <f aca="false">AVERAGE(L19:L28)</f>
+        <v>5.057058</v>
+      </c>
+      <c r="M29" s="0" t="n">
+        <f aca="false">AVERAGE(M19:M28)</f>
+        <v>0.2</v>
+      </c>
+      <c r="N29" s="0" t="n">
+        <f aca="false">AVERAGE(N19:N28)</f>
+        <v>5.344827</v>
+      </c>
+      <c r="O29" s="0" t="n">
+        <f aca="false">AVERAGE(O19:O28)</f>
+        <v>0.3</v>
+      </c>
+    </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="33" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1233,11 +1757,16 @@
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="L2:O2"/>
+  <mergeCells count="2">
+    <mergeCell ref="B2:O2"/>
+    <mergeCell ref="B17:O17"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1269,7 +1798,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -1280,7 +1809,7 @@
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="L1" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
@@ -1293,28 +1822,28 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
       <c r="G2" s="9" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="H2" s="9"/>
       <c r="I2" s="9"/>
       <c r="J2" s="9"/>
       <c r="L2" s="9" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="M2" s="9"/>
       <c r="N2" s="9"/>
       <c r="O2" s="9"/>
       <c r="Q2" s="9" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="R2" s="9"/>
       <c r="S2" s="9"/>
@@ -1325,52 +1854,52 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="M3" s="8" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="R3" s="8" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="T3" s="8" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1381,7 +1910,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D4" s="12" t="n">
         <v>0.065173</v>
@@ -1826,7 +2355,7 @@
         <v>1</v>
       </c>
       <c r="K12" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="L12" s="0" t="n">
         <v>1</v>
@@ -1891,7 +2420,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>1</v>
@@ -1927,41 +2456,41 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D17" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="N17" s="0" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D18" s="0" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="N18" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D19" s="0" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D20" s="0" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="N20" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D21" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -1974,13 +2503,13 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="9" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>
       <c r="E30" s="9"/>
       <c r="G30" s="9" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="H30" s="9"/>
       <c r="I30" s="9"/>
@@ -1991,31 +2520,31 @@
         <v>2</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H31" s="8" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="J31" s="8" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="N31" s="13" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2047,7 +2576,7 @@
         <v>1</v>
       </c>
       <c r="N32" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2108,7 +2637,7 @@
         <v>1</v>
       </c>
       <c r="N34" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2140,7 +2669,7 @@
         <v>1</v>
       </c>
       <c r="N35" s="0" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2172,7 +2701,7 @@
         <v>1</v>
       </c>
       <c r="N36" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2235,7 +2764,7 @@
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="10" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>1</v>
@@ -2313,25 +2842,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
       <c r="F1" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="J1" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
       <c r="N1" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
@@ -2341,40 +2870,40 @@
         <v>2</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="P2" s="8" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2443,25 +2972,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
       <c r="F1" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="J1" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
       <c r="N1" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
@@ -2471,40 +3000,40 @@
         <v>2</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="P2" s="8" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2573,25 +3102,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
       <c r="F1" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="J1" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
       <c r="N1" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
@@ -2601,40 +3130,40 @@
         <v>2</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="P2" s="8" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Added experiment data from Robot Planner 2a with RRTConnect
</commit_message>
<xml_diff>
--- a/data/Thesis Experiments.xlsx
+++ b/data/Thesis Experiments.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="robot_planner1" sheetId="1" state="visible" r:id="rId2"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="56">
   <si>
     <t xml:space="preserve">Robot Planner 1</t>
   </si>
@@ -78,7 +78,47 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t xml:space="preserve">Robot Planner 2</t>
+    <t xml:space="preserve">Robot Planner 2a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trocar1 insertion time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trocar1 reverse 
+Insertion time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Approach trocar2 time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trocar2 insertion time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trocar2 reverse insertion time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Approach trocar3 time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trocar3  insertion time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trocar3 reverse insertion time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Common cause for execution failure is goal tolerance violation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">especially for trocar3 insertion and reverse insertion trajectories which are very close to the</t>
+  </si>
+  <si>
+    <t xml:space="preserve">task space boundary (close to singularities)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Robot Planner 2b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Robot Planner 3b</t>
   </si>
   <si>
     <t xml:space="preserve">RRTConnect</t>
@@ -101,9 +141,6 @@
   <si>
     <t xml:space="preserve">Planning 
 Attempts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Robot Planner 3b</t>
   </si>
   <si>
     <t xml:space="preserve">Robot Planner 4</t>
@@ -180,7 +217,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="#,##0.000000"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -222,6 +259,11 @@
       <name val="Cambria"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Cambria"/>
+      <family val="0"/>
     </font>
     <font>
       <b val="true"/>
@@ -297,7 +339,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -320,6 +362,10 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -350,7 +396,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -426,7 +472,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart39.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -509,11 +555,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="32819758"/>
-        <c:axId val="11885394"/>
+        <c:axId val="89289580"/>
+        <c:axId val="81880229"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="32819758"/>
+        <c:axId val="89289580"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -541,12 +587,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="11885394"/>
+        <c:crossAx val="81880229"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="11885394"/>
+        <c:axId val="81880229"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -583,7 +629,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="32819758"/>
+        <c:crossAx val="89289580"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -673,8 +719,8 @@
   </sheetPr>
   <dimension ref="A2:Q34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M39" activeCellId="0" sqref="M39"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1798,7 +1844,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -1809,7 +1855,7 @@
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="L1" s="2" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
@@ -1822,97 +1868,97 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="G2" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="L2" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-      <c r="Q2" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="R2" s="9"/>
-      <c r="S2" s="9"/>
-      <c r="T2" s="9"/>
+        <v>35</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="G2" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="L2" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="Q2" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="R2" s="10"/>
+      <c r="S2" s="10"/>
+      <c r="T2" s="10"/>
     </row>
     <row r="3" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>19</v>
+      <c r="B3" s="8" t="s">
+        <v>32</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>27</v>
+        <v>38</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>39</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>26</v>
+        <v>32</v>
+      </c>
+      <c r="M3" s="9" t="s">
+        <v>38</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="R3" s="8" t="s">
-        <v>26</v>
+        <v>32</v>
+      </c>
+      <c r="R3" s="9" t="s">
+        <v>38</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="T3" s="8" t="s">
-        <v>21</v>
+        <v>39</v>
+      </c>
+      <c r="T3" s="9" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10" t="n">
+      <c r="A4" s="11" t="n">
         <v>1</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C4" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="12" t="n">
+      <c r="C4" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="13" t="n">
         <v>0.065173</v>
       </c>
       <c r="E4" s="0" t="n">
@@ -1956,7 +2002,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="10" t="n">
+      <c r="A5" s="11" t="n">
         <v>2</v>
       </c>
       <c r="B5" s="0" t="n">
@@ -2009,7 +2055,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="10" t="n">
+      <c r="A6" s="11" t="n">
         <v>3</v>
       </c>
       <c r="B6" s="0" t="n">
@@ -2062,7 +2108,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="10" t="n">
+      <c r="A7" s="11" t="n">
         <v>4</v>
       </c>
       <c r="B7" s="0" t="n">
@@ -2115,7 +2161,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="10" t="n">
+      <c r="A8" s="11" t="n">
         <v>5</v>
       </c>
       <c r="B8" s="0" t="n">
@@ -2168,7 +2214,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="10" t="n">
+      <c r="A9" s="11" t="n">
         <v>6</v>
       </c>
       <c r="B9" s="0" t="n">
@@ -2221,7 +2267,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="10" t="n">
+      <c r="A10" s="11" t="n">
         <v>7</v>
       </c>
       <c r="B10" s="0" t="n">
@@ -2274,7 +2320,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="10" t="n">
+      <c r="A11" s="11" t="n">
         <v>8</v>
       </c>
       <c r="B11" s="0" t="n">
@@ -2327,7 +2373,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="10" t="n">
+      <c r="A12" s="11" t="n">
         <v>9</v>
       </c>
       <c r="B12" s="0" t="n">
@@ -2355,7 +2401,7 @@
         <v>1</v>
       </c>
       <c r="K12" s="0" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="L12" s="0" t="n">
         <v>1</v>
@@ -2390,7 +2436,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="10" t="n">
+      <c r="A13" s="11" t="n">
         <v>10</v>
       </c>
       <c r="B13" s="0" t="n">
@@ -2420,7 +2466,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>1</v>
@@ -2456,41 +2502,41 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D17" s="0" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="N17" s="0" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D18" s="0" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="N18" s="0" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D19" s="0" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D20" s="0" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="N20" s="0" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D21" s="0" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="2" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -2502,53 +2548,53 @@
       <c r="J29" s="2"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="G30" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="H30" s="9"/>
-      <c r="I30" s="9"/>
-      <c r="J30" s="9"/>
+      <c r="B30" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="G30" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
     </row>
     <row r="31" customFormat="false" ht="52.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="7" t="s">
+      <c r="A31" s="8" t="s">
         <v>2</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>26</v>
+        <v>32</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>38</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H31" s="8" t="s">
-        <v>26</v>
+        <v>32</v>
+      </c>
+      <c r="H31" s="9" t="s">
+        <v>38</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="J31" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="N31" s="13" t="s">
         <v>39</v>
       </c>
+      <c r="J31" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="N31" s="14" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="10" t="n">
+      <c r="A32" s="11" t="n">
         <v>1</v>
       </c>
       <c r="B32" s="0" t="n">
@@ -2576,11 +2622,11 @@
         <v>1</v>
       </c>
       <c r="N32" s="0" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="10" t="n">
+      <c r="A33" s="11" t="n">
         <v>2</v>
       </c>
       <c r="B33" s="0" t="n">
@@ -2609,7 +2655,7 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="10" t="n">
+      <c r="A34" s="11" t="n">
         <v>3</v>
       </c>
       <c r="B34" s="0" t="n">
@@ -2637,11 +2683,11 @@
         <v>1</v>
       </c>
       <c r="N34" s="0" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="10" t="n">
+      <c r="A35" s="11" t="n">
         <v>4</v>
       </c>
       <c r="B35" s="0" t="n">
@@ -2669,11 +2715,11 @@
         <v>1</v>
       </c>
       <c r="N35" s="0" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="10" t="n">
+      <c r="A36" s="11" t="n">
         <v>5</v>
       </c>
       <c r="B36" s="0" t="n">
@@ -2701,11 +2747,11 @@
         <v>1</v>
       </c>
       <c r="N36" s="0" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="10" t="n">
+      <c r="A37" s="11" t="n">
         <v>6</v>
       </c>
       <c r="B37" s="0" t="n">
@@ -2734,7 +2780,7 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="10" t="n">
+      <c r="A38" s="11" t="n">
         <v>7</v>
       </c>
       <c r="B38" s="0" t="n">
@@ -2763,8 +2809,8 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="10" t="s">
-        <v>29</v>
+      <c r="A39" s="11" t="s">
+        <v>41</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>1</v>
@@ -2828,120 +2874,914 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P8"/>
+  <dimension ref="A1:T35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N20" activeCellId="0" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.36"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.19"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="F1" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
-      <c r="J1" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
-      <c r="N1" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
-    </row>
-    <row r="2" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+    </row>
+    <row r="2" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="L2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="M2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="N2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="O2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="P2" s="8" t="s">
-        <v>21</v>
+      <c r="R2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="S2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="n">
         <v>1</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>0.060728</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>2.875072</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>2.67618</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>0.168283</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>0.152233</v>
+      </c>
+      <c r="M3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N3" s="0" t="n">
+        <v>0.214332</v>
+      </c>
+      <c r="O3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="0" t="n">
+        <v>0.196175</v>
+      </c>
+      <c r="R3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="S3" s="0" t="n">
+        <v>0.855452</v>
+      </c>
+      <c r="T3" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="n">
         <v>2</v>
       </c>
+      <c r="B4" s="0" t="n">
+        <v>0.070508</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>5.235667</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>5.187283</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>0.179048</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>0.321677</v>
+      </c>
+      <c r="M4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N4" s="0" t="n">
+        <v>0.361712</v>
+      </c>
+      <c r="O4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="0" t="n">
+        <v>0.412455</v>
+      </c>
+      <c r="R4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="S4" s="0" t="n">
+        <v>1.133213</v>
+      </c>
+      <c r="T4" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="n">
         <v>3</v>
       </c>
+      <c r="B5" s="0" t="n">
+        <v>0.071487</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>5.239014</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>0.050117</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>0.057194</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <v>5.404121</v>
+      </c>
+      <c r="M5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N5" s="0" t="n">
+        <v>5.271597</v>
+      </c>
+      <c r="O5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="0" t="n">
+        <v>0.355923</v>
+      </c>
+      <c r="R5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="S5" s="0" t="n">
+        <v>0.814161</v>
+      </c>
+      <c r="T5" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="n">
         <v>4</v>
       </c>
+      <c r="B6" s="0" t="n">
+        <v>0.059288</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>1.733352</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>1.538822</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>0.184641</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L6" s="0" t="n">
+        <v>0.147981</v>
+      </c>
+      <c r="M6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N6" s="0" t="n">
+        <v>0.15915</v>
+      </c>
+      <c r="O6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="0" t="n">
+        <v>0.194839</v>
+      </c>
+      <c r="R6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="S6" s="0" t="n">
+        <v>0.885119</v>
+      </c>
+      <c r="T6" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="n">
         <v>5</v>
       </c>
+      <c r="B7" s="0" t="n">
+        <v>0.053619</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>3.376982</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>1.62114</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>0.253224</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <v>0.333447</v>
+      </c>
+      <c r="M7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N7" s="0" t="n">
+        <v>0.298799</v>
+      </c>
+      <c r="O7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="0" t="n">
+        <v>0.351561</v>
+      </c>
+      <c r="R7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="S7" s="0" t="n">
+        <v>0.364089</v>
+      </c>
+      <c r="T7" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>0.062</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>5.389454</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>5.397757</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>0.268188</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L8" s="0" t="n">
+        <v>0.246624</v>
+      </c>
+      <c r="M8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N8" s="0" t="n">
+        <v>0.209347</v>
+      </c>
+      <c r="O8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="0" t="n">
+        <v>0.355251</v>
+      </c>
+      <c r="R8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="S8" s="0" t="n">
+        <v>0.826636</v>
+      </c>
+      <c r="T8" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>0.084007</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>5.379305</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>0.384924</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L9" s="0" t="n">
+        <v>0.381983</v>
+      </c>
+      <c r="M9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N9" s="0" t="n">
+        <v>0.473779</v>
+      </c>
+      <c r="O9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="0" t="n">
+        <v>0.336123</v>
+      </c>
+      <c r="R9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="S9" s="0" t="n">
+        <v>0.30715</v>
+      </c>
+      <c r="T9" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>0.058306</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>5.254352</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>5.401832</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>0.193265</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L10" s="0" t="n">
+        <v>0.219369</v>
+      </c>
+      <c r="M10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N10" s="0" t="n">
+        <v>0.167211</v>
+      </c>
+      <c r="O10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="0" t="n">
+        <v>0.147867</v>
+      </c>
+      <c r="R10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="S10" s="0" t="n">
+        <v>1.053035</v>
+      </c>
+      <c r="T10" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>0.046925</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>4.90185</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>2.845741</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>0.267069</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L11" s="0" t="n">
+        <v>0.227563</v>
+      </c>
+      <c r="M11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N11" s="0" t="n">
+        <v>0.297372</v>
+      </c>
+      <c r="O11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="0" t="n">
+        <v>0.347956</v>
+      </c>
+      <c r="R11" s="0" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="S11" s="0" t="n">
+        <v>0.80884</v>
+      </c>
+      <c r="T11" s="0" t="n">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>0.060491</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>5.073171</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>5.355111</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>0.250265</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L12" s="0" t="n">
+        <v>5.149372</v>
+      </c>
+      <c r="M12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N12" s="0" t="n">
+        <v>5.3578</v>
+      </c>
+      <c r="O12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="0" t="n">
+        <v>0.28364</v>
+      </c>
+      <c r="R12" s="0" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="S12" s="0" t="n">
+        <v>0.229825</v>
+      </c>
+      <c r="T12" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="B13" s="0" t="n">
+        <f aca="false">AVERAGE(B3:B12)</f>
+        <v>0.0627359</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <f aca="false">AVERAGE(C3:C12)</f>
+        <v>1</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <f aca="false">AVERAGE(D3:D12)</f>
+        <v>4.34210155555556</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <f aca="false">AVERAGE(E3:E12)</f>
+        <v>0.9</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <f aca="false">AVERAGE(G3:G12)</f>
+        <v>3.5453288</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <f aca="false">AVERAGE(H3:H12)</f>
+        <v>1</v>
+      </c>
+      <c r="I13" s="0" t="n">
+        <f aca="false">AVERAGE(I3:I12)</f>
+        <v>0.2206101</v>
+      </c>
+      <c r="J13" s="0" t="n">
+        <f aca="false">AVERAGE(J3:J12)</f>
+        <v>1</v>
+      </c>
+      <c r="L13" s="0" t="n">
+        <f aca="false">AVERAGE(L3:L12)</f>
+        <v>1.258437</v>
+      </c>
+      <c r="M13" s="0" t="n">
+        <f aca="false">AVERAGE(M3:M12)</f>
+        <v>1</v>
+      </c>
+      <c r="N13" s="0" t="n">
+        <f aca="false">AVERAGE(N3:N12)</f>
+        <v>1.2811099</v>
+      </c>
+      <c r="O13" s="0" t="n">
+        <f aca="false">AVERAGE(O3:O12)</f>
+        <v>1</v>
+      </c>
+      <c r="Q13" s="0" t="n">
+        <f aca="false">AVERAGE(Q3:Q12)</f>
+        <v>0.298179</v>
+      </c>
+      <c r="R13" s="0" t="n">
+        <f aca="false">AVERAGE(R3:R12)</f>
+        <v>0.92</v>
+      </c>
+      <c r="S13" s="0" t="n">
+        <f aca="false">AVERAGE(S3:S12)</f>
+        <v>0.727752</v>
+      </c>
+      <c r="T13" s="0" t="n">
+        <f aca="false">AVERAGE(T3:T12)</f>
+        <v>0.237</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O15" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O16" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O17" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2"/>
+      <c r="S23" s="2"/>
+      <c r="T23" s="2"/>
+    </row>
+    <row r="24" customFormat="false" ht="52.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="L24" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M24" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="N24" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="O24" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q24" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="R24" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="S24" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="T24" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="5" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="5" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="5" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="5" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="5" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="5" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="5" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="5" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="5" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35" s="0" t="e">
+        <f aca="false">AVERAGE(B25:B34)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C35" s="0" t="e">
+        <f aca="false">AVERAGE(C25:C34)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D35" s="0" t="e">
+        <f aca="false">AVERAGE(D25:D34)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E35" s="0" t="e">
+        <f aca="false">AVERAGE(E25:E34)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G35" s="0" t="e">
+        <f aca="false">AVERAGE(G25:G34)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H35" s="0" t="e">
+        <f aca="false">AVERAGE(H25:H34)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I35" s="0" t="e">
+        <f aca="false">AVERAGE(I25:I34)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J35" s="0" t="e">
+        <f aca="false">AVERAGE(J25:J34)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L35" s="0" t="e">
+        <f aca="false">AVERAGE(L25:L34)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M35" s="0" t="e">
+        <f aca="false">AVERAGE(M25:M34)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N35" s="0" t="e">
+        <f aca="false">AVERAGE(N25:N34)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O35" s="0" t="e">
+        <f aca="false">AVERAGE(O25:O34)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q35" s="0" t="e">
+        <f aca="false">AVERAGE(Q25:Q34)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R35" s="0" t="e">
+        <f aca="false">AVERAGE(R25:R34)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S35" s="0" t="e">
+        <f aca="false">AVERAGE(S25:S34)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T35" s="0" t="e">
+        <f aca="false">AVERAGE(T25:T34)</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="N1:P1"/>
+  <mergeCells count="2">
+    <mergeCell ref="B1:T1"/>
+    <mergeCell ref="B23:T23"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2972,68 +3812,68 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
+        <v>27</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
       <c r="F1" s="2" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="J1" s="2" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
       <c r="N1" s="2" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="P2" s="8" t="s">
-        <v>21</v>
+      <c r="B2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="P2" s="9" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3102,68 +3942,68 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
+        <v>27</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
       <c r="F1" s="2" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="J1" s="2" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
       <c r="N1" s="2" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="P2" s="8" t="s">
-        <v>21</v>
+      <c r="B2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="P2" s="9" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Bibliography for constrained motion planning, thesis experiments xlsx data update, and write about elbow-up constraint
</commit_message>
<xml_diff>
--- a/data/Thesis Experiments.xlsx
+++ b/data/Thesis Experiments.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="56">
   <si>
     <t xml:space="preserve">Robot Planner 1</t>
   </si>
@@ -472,7 +472,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart39.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart45.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -555,11 +555,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="89289580"/>
-        <c:axId val="81880229"/>
+        <c:axId val="34473146"/>
+        <c:axId val="47927131"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="89289580"/>
+        <c:axId val="34473146"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -587,12 +587,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81880229"/>
+        <c:crossAx val="47927131"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="81880229"/>
+        <c:axId val="47927131"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -629,7 +629,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="89289580"/>
+        <c:crossAx val="34473146"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2876,8 +2876,8 @@
   </sheetPr>
   <dimension ref="A1:T35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N20" activeCellId="0" sqref="N20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q21" activeCellId="0" sqref="Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3663,11 +3663,107 @@
       <c r="A25" s="5" t="n">
         <v>1</v>
       </c>
+      <c r="B25" s="0" t="n">
+        <v>0.076464</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>4.343114</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G25" s="0" t="n">
+        <v>4.94279</v>
+      </c>
+      <c r="H25" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I25" s="0" t="n">
+        <v>0.201385</v>
+      </c>
+      <c r="J25" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L25" s="0" t="n">
+        <v>0.196772</v>
+      </c>
+      <c r="M25" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N25" s="0" t="n">
+        <v>0.351334</v>
+      </c>
+      <c r="O25" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q25" s="0" t="n">
+        <v>0.073863</v>
+      </c>
+      <c r="R25" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="S25" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="T25" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="n">
         <v>2</v>
       </c>
+      <c r="B26" s="0" t="n">
+        <v>0.066101</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>5.236423</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G26" s="0" t="n">
+        <v>5.161566</v>
+      </c>
+      <c r="H26" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I26" s="0" t="n">
+        <v>0.199806</v>
+      </c>
+      <c r="J26" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L26" s="0" t="n">
+        <v>0.185212</v>
+      </c>
+      <c r="M26" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N26" s="0" t="n">
+        <v>0.268024</v>
+      </c>
+      <c r="O26" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q26" s="0" t="n">
+        <v>0.081198</v>
+      </c>
+      <c r="R26" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="S26" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="T26" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="n">
@@ -3713,69 +3809,69 @@
       <c r="A35" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B35" s="0" t="e">
+      <c r="B35" s="0" t="n">
         <f aca="false">AVERAGE(B25:B34)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C35" s="0" t="e">
+        <v>0.0712825</v>
+      </c>
+      <c r="C35" s="0" t="n">
         <f aca="false">AVERAGE(C25:C34)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D35" s="0" t="e">
+        <v>1</v>
+      </c>
+      <c r="D35" s="0" t="n">
         <f aca="false">AVERAGE(D25:D34)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E35" s="0" t="e">
+        <v>4.7897685</v>
+      </c>
+      <c r="E35" s="0" t="n">
         <f aca="false">AVERAGE(E25:E34)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G35" s="0" t="e">
+        <v>1</v>
+      </c>
+      <c r="G35" s="0" t="n">
         <f aca="false">AVERAGE(G25:G34)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H35" s="0" t="e">
+        <v>5.052178</v>
+      </c>
+      <c r="H35" s="0" t="n">
         <f aca="false">AVERAGE(H25:H34)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I35" s="0" t="e">
+        <v>1</v>
+      </c>
+      <c r="I35" s="0" t="n">
         <f aca="false">AVERAGE(I25:I34)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J35" s="0" t="e">
+        <v>0.2005955</v>
+      </c>
+      <c r="J35" s="0" t="n">
         <f aca="false">AVERAGE(J25:J34)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L35" s="0" t="e">
+        <v>1</v>
+      </c>
+      <c r="L35" s="0" t="n">
         <f aca="false">AVERAGE(L25:L34)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M35" s="0" t="e">
+        <v>0.190992</v>
+      </c>
+      <c r="M35" s="0" t="n">
         <f aca="false">AVERAGE(M25:M34)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N35" s="0" t="e">
+        <v>1</v>
+      </c>
+      <c r="N35" s="0" t="n">
         <f aca="false">AVERAGE(N25:N34)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O35" s="0" t="e">
+        <v>0.309679</v>
+      </c>
+      <c r="O35" s="0" t="n">
         <f aca="false">AVERAGE(O25:O34)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q35" s="0" t="e">
+        <v>1</v>
+      </c>
+      <c r="Q35" s="0" t="n">
         <f aca="false">AVERAGE(Q25:Q34)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R35" s="0" t="e">
+        <v>0.0775305</v>
+      </c>
+      <c r="R35" s="0" t="n">
         <f aca="false">AVERAGE(R25:R34)</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="S35" s="0" t="e">
         <f aca="false">AVERAGE(S25:S34)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="T35" s="0" t="e">
+      <c r="T35" s="0" t="n">
         <f aca="false">AVERAGE(T25:T34)</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added experiment data from robot_planner2b
</commit_message>
<xml_diff>
--- a/data/Thesis Experiments.xlsx
+++ b/data/Thesis Experiments.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="56">
   <si>
     <t xml:space="preserve">Robot Planner 1</t>
   </si>
@@ -217,7 +217,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="#,##0.000000"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -259,11 +259,6 @@
       <name val="Cambria"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Cambria"/>
-      <family val="0"/>
     </font>
     <font>
       <b val="true"/>
@@ -339,7 +334,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -362,10 +357,6 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -396,7 +387,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -472,7 +463,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -555,11 +546,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="34473146"/>
-        <c:axId val="47927131"/>
+        <c:axId val="33012732"/>
+        <c:axId val="96633658"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="34473146"/>
+        <c:axId val="33012732"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -587,12 +578,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="47927131"/>
+        <c:crossAx val="96633658"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="47927131"/>
+        <c:axId val="96633658"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -629,7 +620,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="34473146"/>
+        <c:crossAx val="33012732"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -688,9 +679,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>98640</xdr:colOff>
+      <xdr:colOff>98280</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>153360</xdr:rowOff>
+      <xdr:rowOff>153000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -699,7 +690,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="10197000" y="9605520"/>
-        <a:ext cx="5756760" cy="3236400"/>
+        <a:ext cx="5756400" cy="3236040"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1870,36 +1861,36 @@
       <c r="A2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="G2" s="10" t="s">
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="G2" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="L2" s="10" t="s">
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="L2" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="Q2" s="10" t="s">
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="Q2" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="R2" s="10"/>
-      <c r="S2" s="10"/>
-      <c r="T2" s="10"/>
+      <c r="R2" s="9"/>
+      <c r="S2" s="9"/>
+      <c r="T2" s="9"/>
     </row>
     <row r="3" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>32</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -1917,7 +1908,7 @@
       <c r="H3" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="8" t="s">
         <v>39</v>
       </c>
       <c r="J3" s="4" t="s">
@@ -1926,7 +1917,7 @@
       <c r="L3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="M3" s="9" t="s">
+      <c r="M3" s="8" t="s">
         <v>38</v>
       </c>
       <c r="N3" s="4" t="s">
@@ -1938,27 +1929,27 @@
       <c r="Q3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="R3" s="9" t="s">
+      <c r="R3" s="8" t="s">
         <v>38</v>
       </c>
       <c r="S3" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="T3" s="9" t="s">
+      <c r="T3" s="8" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="11" t="n">
+      <c r="A4" s="10" t="n">
         <v>1</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D4" s="13" t="n">
+      <c r="D4" s="12" t="n">
         <v>0.065173</v>
       </c>
       <c r="E4" s="0" t="n">
@@ -2002,7 +1993,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="11" t="n">
+      <c r="A5" s="10" t="n">
         <v>2</v>
       </c>
       <c r="B5" s="0" t="n">
@@ -2055,7 +2046,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="11" t="n">
+      <c r="A6" s="10" t="n">
         <v>3</v>
       </c>
       <c r="B6" s="0" t="n">
@@ -2108,7 +2099,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="11" t="n">
+      <c r="A7" s="10" t="n">
         <v>4</v>
       </c>
       <c r="B7" s="0" t="n">
@@ -2161,7 +2152,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="11" t="n">
+      <c r="A8" s="10" t="n">
         <v>5</v>
       </c>
       <c r="B8" s="0" t="n">
@@ -2214,7 +2205,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="11" t="n">
+      <c r="A9" s="10" t="n">
         <v>6</v>
       </c>
       <c r="B9" s="0" t="n">
@@ -2267,7 +2258,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="11" t="n">
+      <c r="A10" s="10" t="n">
         <v>7</v>
       </c>
       <c r="B10" s="0" t="n">
@@ -2320,7 +2311,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="11" t="n">
+      <c r="A11" s="10" t="n">
         <v>8</v>
       </c>
       <c r="B11" s="0" t="n">
@@ -2373,7 +2364,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="11" t="n">
+      <c r="A12" s="10" t="n">
         <v>9</v>
       </c>
       <c r="B12" s="0" t="n">
@@ -2436,7 +2427,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="11" t="n">
+      <c r="A13" s="10" t="n">
         <v>10</v>
       </c>
       <c r="B13" s="0" t="n">
@@ -2548,27 +2539,27 @@
       <c r="J29" s="2"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-      <c r="G30" s="10" t="s">
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="G30" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="H30" s="10"/>
-      <c r="I30" s="10"/>
-      <c r="J30" s="10"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
     </row>
     <row r="31" customFormat="false" ht="52.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="8" t="s">
+      <c r="A31" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="C31" s="8" t="s">
         <v>38</v>
       </c>
       <c r="D31" s="4" t="s">
@@ -2580,21 +2571,21 @@
       <c r="G31" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="H31" s="9" t="s">
+      <c r="H31" s="8" t="s">
         <v>38</v>
       </c>
       <c r="I31" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="J31" s="9" t="s">
+      <c r="J31" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="N31" s="14" t="s">
+      <c r="N31" s="13" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="11" t="n">
+      <c r="A32" s="10" t="n">
         <v>1</v>
       </c>
       <c r="B32" s="0" t="n">
@@ -2626,7 +2617,7 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="11" t="n">
+      <c r="A33" s="10" t="n">
         <v>2</v>
       </c>
       <c r="B33" s="0" t="n">
@@ -2655,7 +2646,7 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="11" t="n">
+      <c r="A34" s="10" t="n">
         <v>3</v>
       </c>
       <c r="B34" s="0" t="n">
@@ -2687,7 +2678,7 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="11" t="n">
+      <c r="A35" s="10" t="n">
         <v>4</v>
       </c>
       <c r="B35" s="0" t="n">
@@ -2719,7 +2710,7 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="11" t="n">
+      <c r="A36" s="10" t="n">
         <v>5</v>
       </c>
       <c r="B36" s="0" t="n">
@@ -2751,7 +2742,7 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="11" t="n">
+      <c r="A37" s="10" t="n">
         <v>6</v>
       </c>
       <c r="B37" s="0" t="n">
@@ -2780,7 +2771,7 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="11" t="n">
+      <c r="A38" s="10" t="n">
         <v>7</v>
       </c>
       <c r="B38" s="0" t="n">
@@ -2809,7 +2800,7 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="11" t="s">
+      <c r="A39" s="10" t="s">
         <v>41</v>
       </c>
       <c r="B39" s="0" t="n">
@@ -2876,8 +2867,8 @@
   </sheetPr>
   <dimension ref="A1:T35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q21" activeCellId="0" sqref="Q21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T39" activeCellId="0" sqref="T39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2959,7 +2950,7 @@
       <c r="R2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="S2" s="6" t="s">
+      <c r="S2" s="4" t="s">
         <v>22</v>
       </c>
       <c r="T2" s="4" t="s">
@@ -3652,7 +3643,7 @@
       <c r="R24" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="S24" s="6" t="s">
+      <c r="S24" s="4" t="s">
         <v>22</v>
       </c>
       <c r="T24" s="4" t="s">
@@ -3664,52 +3655,53 @@
         <v>1</v>
       </c>
       <c r="B25" s="0" t="n">
-        <v>0.076464</v>
+        <v>0.269901</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D25" s="0" t="n">
-        <v>4.343114</v>
+        <v>0.355588</v>
       </c>
       <c r="E25" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G25" s="0" t="n">
-        <v>4.94279</v>
+        <v>0.322578</v>
       </c>
       <c r="H25" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I25" s="0" t="n">
-        <v>0.201385</v>
+        <v>0.283497</v>
       </c>
       <c r="J25" s="0" t="n">
         <v>1</v>
       </c>
       <c r="L25" s="0" t="n">
-        <v>0.196772</v>
+        <v>5.374646</v>
       </c>
       <c r="M25" s="0" t="n">
         <v>1</v>
       </c>
       <c r="N25" s="0" t="n">
-        <v>0.351334</v>
+        <f aca="false">5.393437+0.057898</f>
+        <v>5.451335</v>
       </c>
       <c r="O25" s="0" t="n">
         <v>1</v>
       </c>
       <c r="Q25" s="0" t="n">
-        <v>0.073863</v>
+        <v>0.372382</v>
       </c>
       <c r="R25" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="S25" s="0" t="s">
-        <v>10</v>
+      <c r="S25" s="0" t="n">
+        <v>5.34059</v>
       </c>
       <c r="T25" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3717,93 +3709,486 @@
         <v>2</v>
       </c>
       <c r="B26" s="0" t="n">
-        <v>0.066101</v>
+        <v>0.220509</v>
       </c>
       <c r="C26" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D26" s="0" t="n">
-        <v>5.236423</v>
+        <v>0.255968</v>
       </c>
       <c r="E26" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G26" s="0" t="n">
-        <v>5.161566</v>
+        <v>0.209871</v>
       </c>
       <c r="H26" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I26" s="0" t="n">
-        <v>0.199806</v>
+        <v>0.410543</v>
       </c>
       <c r="J26" s="0" t="n">
         <v>1</v>
       </c>
       <c r="L26" s="0" t="n">
-        <v>0.185212</v>
+        <v>0.452231</v>
       </c>
       <c r="M26" s="0" t="n">
         <v>1</v>
       </c>
       <c r="N26" s="0" t="n">
-        <v>0.268024</v>
+        <f aca="false">0.194387+0.059282</f>
+        <v>0.253669</v>
       </c>
       <c r="O26" s="0" t="n">
         <v>1</v>
       </c>
       <c r="Q26" s="0" t="n">
-        <v>0.081198</v>
+        <v>0.280432</v>
       </c>
       <c r="R26" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="S26" s="0" t="s">
-        <v>10</v>
+      <c r="S26" s="0" t="n">
+        <v>0.261765</v>
       </c>
       <c r="T26" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="n">
         <v>3</v>
       </c>
+      <c r="B27" s="0" t="n">
+        <v>0.260483</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>5.28604</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G27" s="0" t="n">
+        <v>5.099769</v>
+      </c>
+      <c r="H27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I27" s="0" t="n">
+        <v>0.296228</v>
+      </c>
+      <c r="J27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L27" s="0" t="n">
+        <v>0.22638</v>
+      </c>
+      <c r="M27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N27" s="0" t="n">
+        <f aca="false">0.31488+0.069053</f>
+        <v>0.383933</v>
+      </c>
+      <c r="O27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q27" s="0" t="n">
+        <v>0.179581</v>
+      </c>
+      <c r="R27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="S27" s="0" t="n">
+        <v>0.187589</v>
+      </c>
+      <c r="T27" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="n">
         <v>4</v>
       </c>
+      <c r="B28" s="0" t="n">
+        <v>0.267778</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>0.267796</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G28" s="0" t="n">
+        <v>0.216997</v>
+      </c>
+      <c r="H28" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I28" s="0" t="n">
+        <v>0.342776</v>
+      </c>
+      <c r="J28" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L28" s="0" t="n">
+        <v>5.371822</v>
+      </c>
+      <c r="M28" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N28" s="0" t="n">
+        <f aca="false">5.525819+0.08583</f>
+        <v>5.611649</v>
+      </c>
+      <c r="O28" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q28" s="0" t="n">
+        <v>0.121094</v>
+      </c>
+      <c r="R28" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="S28" s="0" t="n">
+        <v>5.152808</v>
+      </c>
+      <c r="T28" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5" t="n">
         <v>5</v>
       </c>
+      <c r="B29" s="0" t="n">
+        <v>0.388487</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>5.321684</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G29" s="0" t="n">
+        <v>5.328204</v>
+      </c>
+      <c r="H29" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I29" s="0" t="n">
+        <v>0.394472</v>
+      </c>
+      <c r="J29" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L29" s="0" t="n">
+        <v>0.395787</v>
+      </c>
+      <c r="M29" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N29" s="0" t="n">
+        <f aca="false">0.240031+0.069181</f>
+        <v>0.309212</v>
+      </c>
+      <c r="O29" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q29" s="0" t="n">
+        <v>0.472468</v>
+      </c>
+      <c r="R29" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="S29" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="T29" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="n">
         <v>6</v>
       </c>
+      <c r="B30" s="0" t="n">
+        <v>0.316275</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>0.2088</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G30" s="0" t="n">
+        <v>0.450936</v>
+      </c>
+      <c r="H30" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I30" s="0" t="n">
+        <v>0.249248</v>
+      </c>
+      <c r="J30" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L30" s="0" t="n">
+        <v>5.15406</v>
+      </c>
+      <c r="M30" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N30" s="0" t="n">
+        <f aca="false">5.453679+0.061328</f>
+        <v>5.515007</v>
+      </c>
+      <c r="O30" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q30" s="0" t="n">
+        <v>0.251195</v>
+      </c>
+      <c r="R30" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="S30" s="0" t="n">
+        <v>0.442282</v>
+      </c>
+      <c r="T30" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="5" t="n">
         <v>7</v>
       </c>
+      <c r="B31" s="0" t="n">
+        <v>0.202614</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>0.14469</v>
+      </c>
+      <c r="E31" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G31" s="0" t="n">
+        <v>0.336209</v>
+      </c>
+      <c r="H31" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I31" s="0" t="n">
+        <v>0.165375</v>
+      </c>
+      <c r="J31" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L31" s="0" t="n">
+        <v>4.189377</v>
+      </c>
+      <c r="M31" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N31" s="0" t="n">
+        <f aca="false">5.509548+0.06102</f>
+        <v>5.570568</v>
+      </c>
+      <c r="O31" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q31" s="0" t="n">
+        <v>0.20647</v>
+      </c>
+      <c r="R31" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="S31" s="0" t="n">
+        <v>0.318481</v>
+      </c>
+      <c r="T31" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5" t="n">
         <v>8</v>
       </c>
+      <c r="B32" s="0" t="n">
+        <v>0.289368</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>0.275917</v>
+      </c>
+      <c r="E32" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G32" s="0" t="n">
+        <v>0.397699</v>
+      </c>
+      <c r="H32" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I32" s="0" t="n">
+        <v>0.202118</v>
+      </c>
+      <c r="J32" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L32" s="0" t="n">
+        <v>5.167346</v>
+      </c>
+      <c r="M32" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N32" s="0" t="n">
+        <f aca="false">5.446353+0.075703</f>
+        <v>5.522056</v>
+      </c>
+      <c r="O32" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q32" s="0" t="n">
+        <v>0.178941</v>
+      </c>
+      <c r="R32" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="S32" s="0" t="n">
+        <v>0.185758</v>
+      </c>
+      <c r="T32" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="5" t="n">
         <v>9</v>
       </c>
+      <c r="B33" s="0" t="n">
+        <v>0.353631</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>0.353631</v>
+      </c>
+      <c r="E33" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G33" s="0" t="n">
+        <v>0.235555</v>
+      </c>
+      <c r="H33" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I33" s="0" t="n">
+        <v>0.333129</v>
+      </c>
+      <c r="J33" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L33" s="0" t="n">
+        <v>5.101735</v>
+      </c>
+      <c r="M33" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N33" s="0" t="n">
+        <f aca="false">5.388814+0.063487</f>
+        <v>5.452301</v>
+      </c>
+      <c r="O33" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q33" s="0" t="n">
+        <v>0.188906</v>
+      </c>
+      <c r="R33" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="S33" s="0" t="n">
+        <v>0.222821</v>
+      </c>
+      <c r="T33" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="5" t="n">
         <v>10</v>
       </c>
+      <c r="B34" s="0" t="n">
+        <v>0.185345</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>0.154755</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G34" s="0" t="n">
+        <v>0.320059</v>
+      </c>
+      <c r="H34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I34" s="0" t="n">
+        <v>0.343595</v>
+      </c>
+      <c r="J34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L34" s="0" t="n">
+        <v>5.273342</v>
+      </c>
+      <c r="M34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N34" s="0" t="n">
+        <f aca="false">5.40755+0.059723</f>
+        <v>5.467273</v>
+      </c>
+      <c r="O34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q34" s="0" t="n">
+        <v>0.165681</v>
+      </c>
+      <c r="R34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="S34" s="0" t="n">
+        <v>0.170876</v>
+      </c>
+      <c r="T34" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
@@ -3811,7 +4196,7 @@
       </c>
       <c r="B35" s="0" t="n">
         <f aca="false">AVERAGE(B25:B34)</f>
-        <v>0.0712825</v>
+        <v>0.2754391</v>
       </c>
       <c r="C35" s="0" t="n">
         <f aca="false">AVERAGE(C25:C34)</f>
@@ -3819,7 +4204,7 @@
       </c>
       <c r="D35" s="0" t="n">
         <f aca="false">AVERAGE(D25:D34)</f>
-        <v>4.7897685</v>
+        <v>1.2624869</v>
       </c>
       <c r="E35" s="0" t="n">
         <f aca="false">AVERAGE(E25:E34)</f>
@@ -3827,7 +4212,7 @@
       </c>
       <c r="G35" s="0" t="n">
         <f aca="false">AVERAGE(G25:G34)</f>
-        <v>5.052178</v>
+        <v>1.2917877</v>
       </c>
       <c r="H35" s="0" t="n">
         <f aca="false">AVERAGE(H25:H34)</f>
@@ -3835,7 +4220,7 @@
       </c>
       <c r="I35" s="0" t="n">
         <f aca="false">AVERAGE(I25:I34)</f>
-        <v>0.2005955</v>
+        <v>0.3020981</v>
       </c>
       <c r="J35" s="0" t="n">
         <f aca="false">AVERAGE(J25:J34)</f>
@@ -3843,7 +4228,7 @@
       </c>
       <c r="L35" s="0" t="n">
         <f aca="false">AVERAGE(L25:L34)</f>
-        <v>0.190992</v>
+        <v>3.6706726</v>
       </c>
       <c r="M35" s="0" t="n">
         <f aca="false">AVERAGE(M25:M34)</f>
@@ -3851,7 +4236,7 @@
       </c>
       <c r="N35" s="0" t="n">
         <f aca="false">AVERAGE(N25:N34)</f>
-        <v>0.309679</v>
+        <v>3.9537003</v>
       </c>
       <c r="O35" s="0" t="n">
         <f aca="false">AVERAGE(O25:O34)</f>
@@ -3859,19 +4244,19 @@
       </c>
       <c r="Q35" s="0" t="n">
         <f aca="false">AVERAGE(Q25:Q34)</f>
-        <v>0.0775305</v>
+        <v>0.241715</v>
       </c>
       <c r="R35" s="0" t="n">
         <f aca="false">AVERAGE(R25:R34)</f>
         <v>1</v>
       </c>
-      <c r="S35" s="0" t="e">
+      <c r="S35" s="0" t="n">
         <f aca="false">AVERAGE(S25:S34)</f>
-        <v>#DIV/0!</v>
+        <v>1.36477444444444</v>
       </c>
       <c r="T35" s="0" t="n">
         <f aca="false">AVERAGE(T25:T34)</f>
-        <v>0</v>
+        <v>0.8</v>
       </c>
     </row>
   </sheetData>
@@ -3910,11 +4295,11 @@
       <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
       <c r="F1" s="2" t="s">
         <v>29</v>
       </c>
@@ -3932,43 +4317,43 @@
       <c r="P1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="L2" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="N2" s="8" t="s">
+      <c r="N2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="O2" s="8" t="s">
+      <c r="O2" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="P2" s="8" t="s">
         <v>34</v>
       </c>
     </row>
@@ -4040,11 +4425,11 @@
       <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
       <c r="F1" s="2" t="s">
         <v>29</v>
       </c>
@@ -4062,43 +4447,43 @@
       <c r="P1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="L2" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="N2" s="8" t="s">
+      <c r="N2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="O2" s="8" t="s">
+      <c r="O2" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="P2" s="8" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Replaces screenshots for robot_planners 3a and 3b and added rcm error diagrams for 3b as well as experiment data in excel spreadsheet
</commit_message>
<xml_diff>
--- a/data/Thesis Experiments.xlsx
+++ b/data/Thesis Experiments.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="robot_planner1" sheetId="1" state="visible" r:id="rId2"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="67">
   <si>
     <t xml:space="preserve">Robot Planner 1</t>
   </si>
@@ -141,6 +141,47 @@
   <si>
     <t xml:space="preserve">Planning 
 Attempts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elbow-up 
+Start pose 
+planning time (sec)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elbow-up preparation path planning time (sec)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Approach fulcrum 2
+Path planning time
+(sec)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insertion path planning time (sec)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Line segment 
+Path planning time (sec)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reverse line segment
+Path planning time (sec)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Line segment trajectory 
+Calculation time
+(micro seconds)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">starting from home position</t>
+  </si>
+  <si>
+    <t xml:space="preserve">in pivot line segment trajectory could avoid moveit path planning!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mention system specifications</t>
   </si>
   <si>
     <t xml:space="preserve">Robot Planner 4</t>
@@ -217,7 +258,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="#,##0.000000"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -261,6 +302,12 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -274,7 +321,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -296,16 +343,78 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF93C47D"/>
-        <bgColor rgb="FFB3B3B3"/>
+        <bgColor rgb="FF72BF44"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF72BF44"/>
+        <bgColor rgb="FF93C47D"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="hair"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
   </borders>
@@ -334,7 +443,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -372,6 +481,58 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -387,7 +548,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -444,7 +605,7 @@
       <rgbColor rgb="FFF9CB9C"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FF72BF44"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
@@ -463,7 +624,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -546,11 +707,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="13868025"/>
-        <c:axId val="63855338"/>
+        <c:axId val="65635503"/>
+        <c:axId val="67650826"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="13868025"/>
+        <c:axId val="65635503"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -578,12 +739,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="63855338"/>
+        <c:crossAx val="67650826"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="63855338"/>
+        <c:axId val="67650826"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -620,7 +781,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="13868025"/>
+        <c:crossAx val="65635503"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -679,9 +840,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>98280</xdr:colOff>
+      <xdr:colOff>97920</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>153000</xdr:rowOff>
+      <xdr:rowOff>152640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -690,7 +851,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="10197000" y="9605520"/>
-        <a:ext cx="5756400" cy="3236040"/>
+        <a:ext cx="5756040" cy="3235680"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -711,7 +872,7 @@
   <dimension ref="A2:Q34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1859,32 +2020,32 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="G2" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="L2" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-      <c r="Q2" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="R2" s="9"/>
-      <c r="S2" s="9"/>
-      <c r="T2" s="9"/>
+        <v>46</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="G2" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="L2" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
+      <c r="Q2" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="R2" s="22"/>
+      <c r="S2" s="22"/>
+      <c r="T2" s="22"/>
     </row>
     <row r="3" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
@@ -1894,10 +2055,10 @@
         <v>32</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>34</v>
@@ -1906,10 +2067,10 @@
         <v>32</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>34</v>
@@ -1918,10 +2079,10 @@
         <v>32</v>
       </c>
       <c r="M3" s="8" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="O3" s="4" t="s">
         <v>34</v>
@@ -1930,26 +2091,26 @@
         <v>32</v>
       </c>
       <c r="R3" s="8" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="T3" s="8" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10" t="n">
+      <c r="A4" s="23" t="n">
         <v>1</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C4" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="12" t="n">
+      <c r="C4" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="25" t="n">
         <v>0.065173</v>
       </c>
       <c r="E4" s="0" t="n">
@@ -1993,7 +2154,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="10" t="n">
+      <c r="A5" s="23" t="n">
         <v>2</v>
       </c>
       <c r="B5" s="0" t="n">
@@ -2046,7 +2207,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="10" t="n">
+      <c r="A6" s="23" t="n">
         <v>3</v>
       </c>
       <c r="B6" s="0" t="n">
@@ -2099,7 +2260,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="10" t="n">
+      <c r="A7" s="23" t="n">
         <v>4</v>
       </c>
       <c r="B7" s="0" t="n">
@@ -2152,7 +2313,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="10" t="n">
+      <c r="A8" s="23" t="n">
         <v>5</v>
       </c>
       <c r="B8" s="0" t="n">
@@ -2205,7 +2366,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="10" t="n">
+      <c r="A9" s="23" t="n">
         <v>6</v>
       </c>
       <c r="B9" s="0" t="n">
@@ -2258,7 +2419,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="10" t="n">
+      <c r="A10" s="23" t="n">
         <v>7</v>
       </c>
       <c r="B10" s="0" t="n">
@@ -2311,7 +2472,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="10" t="n">
+      <c r="A11" s="23" t="n">
         <v>8</v>
       </c>
       <c r="B11" s="0" t="n">
@@ -2364,7 +2525,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="10" t="n">
+      <c r="A12" s="23" t="n">
         <v>9</v>
       </c>
       <c r="B12" s="0" t="n">
@@ -2392,7 +2553,7 @@
         <v>1</v>
       </c>
       <c r="K12" s="0" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="L12" s="0" t="n">
         <v>1</v>
@@ -2427,7 +2588,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="10" t="n">
+      <c r="A13" s="23" t="n">
         <v>10</v>
       </c>
       <c r="B13" s="0" t="n">
@@ -2457,7 +2618,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>1</v>
@@ -2493,36 +2654,36 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D17" s="0" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="N17" s="0" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D18" s="0" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="N18" s="0" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D19" s="0" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D20" s="0" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="N20" s="0" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D21" s="0" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2539,18 +2700,18 @@
       <c r="J29" s="2"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="G30" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="H30" s="9"/>
-      <c r="I30" s="9"/>
-      <c r="J30" s="9"/>
+      <c r="B30" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="G30" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="H30" s="22"/>
+      <c r="I30" s="22"/>
+      <c r="J30" s="22"/>
     </row>
     <row r="31" customFormat="false" ht="52.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="7" t="s">
@@ -2560,10 +2721,10 @@
         <v>32</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>34</v>
@@ -2572,20 +2733,20 @@
         <v>32</v>
       </c>
       <c r="H31" s="8" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="J31" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="N31" s="13" t="s">
-        <v>51</v>
+      <c r="N31" s="26" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="10" t="n">
+      <c r="A32" s="23" t="n">
         <v>1</v>
       </c>
       <c r="B32" s="0" t="n">
@@ -2613,11 +2774,11 @@
         <v>1</v>
       </c>
       <c r="N32" s="0" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="10" t="n">
+      <c r="A33" s="23" t="n">
         <v>2</v>
       </c>
       <c r="B33" s="0" t="n">
@@ -2646,7 +2807,7 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="10" t="n">
+      <c r="A34" s="23" t="n">
         <v>3</v>
       </c>
       <c r="B34" s="0" t="n">
@@ -2674,11 +2835,11 @@
         <v>1</v>
       </c>
       <c r="N34" s="0" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="10" t="n">
+      <c r="A35" s="23" t="n">
         <v>4</v>
       </c>
       <c r="B35" s="0" t="n">
@@ -2706,11 +2867,11 @@
         <v>1</v>
       </c>
       <c r="N35" s="0" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="10" t="n">
+      <c r="A36" s="23" t="n">
         <v>5</v>
       </c>
       <c r="B36" s="0" t="n">
@@ -2738,11 +2899,11 @@
         <v>1</v>
       </c>
       <c r="N36" s="0" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="10" t="n">
+      <c r="A37" s="23" t="n">
         <v>6</v>
       </c>
       <c r="B37" s="0" t="n">
@@ -2771,7 +2932,7 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="10" t="n">
+      <c r="A38" s="23" t="n">
         <v>7</v>
       </c>
       <c r="B38" s="0" t="n">
@@ -2800,8 +2961,8 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="10" t="s">
-        <v>41</v>
+      <c r="A39" s="23" t="s">
+        <v>52</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>1</v>
@@ -2867,7 +3028,7 @@
   </sheetPr>
   <dimension ref="A1:T35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="T9" activeCellId="0" sqref="T9"/>
     </sheetView>
   </sheetViews>
@@ -4409,120 +4570,610 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P8"/>
+  <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I23" activeCellId="0" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.7"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="6.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="6.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="23.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="6.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="6.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="0" width="23.06"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="16" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="F1" s="2" t="s">
-        <v>29</v>
-      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
-      <c r="J1" s="2" t="s">
-        <v>30</v>
-      </c>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
-      <c r="N1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-    </row>
-    <row r="2" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
+      <c r="M1" s="2"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+    </row>
+    <row r="2" customFormat="false" ht="65.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2" s="7" t="s">
+      <c r="D2" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="J2" s="7" t="s">
+      <c r="F2" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="K2" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="N2" s="7" t="s">
+      <c r="H2" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="O2" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="P2" s="8" t="s">
-        <v>34</v>
-      </c>
+      <c r="J2" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="M2" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="P2" s="15"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="n">
-        <v>1</v>
+      <c r="A3" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>0.221091</v>
+      </c>
+      <c r="C3" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>0.074075</v>
+      </c>
+      <c r="E3" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>0.067982</v>
+      </c>
+      <c r="G3" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>0.30244</v>
+      </c>
+      <c r="I3" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>5.326128</v>
+      </c>
+      <c r="K3" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>5.486623</v>
+      </c>
+      <c r="M3" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="N3" s="17" t="n">
+        <v>684</v>
+      </c>
+      <c r="P3" s="0" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="n">
+      <c r="A4" s="16" t="n">
         <v>2</v>
       </c>
+      <c r="B4" s="0" t="n">
+        <v>0.19466</v>
+      </c>
+      <c r="C4" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>0.194823</v>
+      </c>
+      <c r="E4" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>0.345301</v>
+      </c>
+      <c r="G4" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>0.325638</v>
+      </c>
+      <c r="I4" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>0.479823</v>
+      </c>
+      <c r="K4" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>5.279854</v>
+      </c>
+      <c r="M4" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="N4" s="17" t="n">
+        <v>584</v>
+      </c>
+      <c r="P4" s="0" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="n">
+      <c r="A5" s="16" t="n">
         <v>3</v>
       </c>
+      <c r="B5" s="0" t="n">
+        <v>0.268828</v>
+      </c>
+      <c r="C5" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>0.073928</v>
+      </c>
+      <c r="E5" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>0.112407</v>
+      </c>
+      <c r="G5" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>0.173074</v>
+      </c>
+      <c r="I5" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>0.288405</v>
+      </c>
+      <c r="K5" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="L5" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="M5" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" s="17" t="n">
+        <v>339</v>
+      </c>
+      <c r="P5" s="18" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="n">
+      <c r="A6" s="16" t="n">
         <v>4</v>
       </c>
+      <c r="B6" s="0" t="n">
+        <v>0.154783</v>
+      </c>
+      <c r="C6" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>0.049908</v>
+      </c>
+      <c r="E6" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>0.054112</v>
+      </c>
+      <c r="G6" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>0.194001</v>
+      </c>
+      <c r="I6" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>0.295343</v>
+      </c>
+      <c r="K6" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="M6" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" s="17" t="n">
+        <v>341</v>
+      </c>
+      <c r="P6" s="0" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="n">
+      <c r="A7" s="16" t="n">
         <v>5</v>
       </c>
+      <c r="B7" s="0" t="n">
+        <v>0.110496</v>
+      </c>
+      <c r="C7" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>0.104181</v>
+      </c>
+      <c r="E7" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>0.117048</v>
+      </c>
+      <c r="G7" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>0.23512</v>
+      </c>
+      <c r="I7" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>0.225066</v>
+      </c>
+      <c r="K7" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <v>5.445483</v>
+      </c>
+      <c r="M7" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="N7" s="17" t="n">
+        <v>504</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="16" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>0.155316</v>
+      </c>
+      <c r="C8" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>0.061127</v>
+      </c>
+      <c r="E8" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>0.055864</v>
+      </c>
+      <c r="G8" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>0.284625</v>
+      </c>
+      <c r="I8" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>5.132968</v>
+      </c>
+      <c r="K8" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="L8" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="M8" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" s="17" t="n">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="16" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>0.140189</v>
+      </c>
+      <c r="C9" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>0.048735</v>
+      </c>
+      <c r="E9" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>0.07501</v>
+      </c>
+      <c r="G9" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>0.231642</v>
+      </c>
+      <c r="I9" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>0.300322</v>
+      </c>
+      <c r="K9" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="L9" s="0" t="n">
+        <v>5.285311</v>
+      </c>
+      <c r="M9" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="N9" s="17" t="n">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="16" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>0.166412</v>
+      </c>
+      <c r="C10" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>0.261208</v>
+      </c>
+      <c r="E10" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>0.170249</v>
+      </c>
+      <c r="G10" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>0.105259</v>
+      </c>
+      <c r="I10" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>5.484813</v>
+      </c>
+      <c r="K10" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="L10" s="0" t="n">
+        <v>5.403696</v>
+      </c>
+      <c r="M10" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="N10" s="17" t="n">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="16" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>0.121243</v>
+      </c>
+      <c r="C11" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>0.247453</v>
+      </c>
+      <c r="E11" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>0.102762</v>
+      </c>
+      <c r="G11" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>0.374426</v>
+      </c>
+      <c r="I11" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>0.297406</v>
+      </c>
+      <c r="K11" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="L11" s="0" t="n">
+        <v>5.309383</v>
+      </c>
+      <c r="M11" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="N11" s="17" t="n">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="19" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" s="20" t="n">
+        <v>0.209206</v>
+      </c>
+      <c r="C12" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" s="20" t="n">
+        <v>0.054966</v>
+      </c>
+      <c r="E12" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" s="20" t="n">
+        <v>0.064243</v>
+      </c>
+      <c r="G12" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="H12" s="20" t="n">
+        <v>0.269333</v>
+      </c>
+      <c r="I12" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="J12" s="20" t="n">
+        <v>0.259739</v>
+      </c>
+      <c r="K12" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="L12" s="20" t="n">
+        <v>5.285902</v>
+      </c>
+      <c r="M12" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="N12" s="21" t="n">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="19" t="s">
         <v>11</v>
       </c>
+      <c r="B13" s="20" t="n">
+        <f aca="false">AVERAGE(B3:B12)</f>
+        <v>0.1742224</v>
+      </c>
+      <c r="C13" s="20" t="n">
+        <f aca="false">AVERAGE(C3:C12)</f>
+        <v>1</v>
+      </c>
+      <c r="D13" s="20" t="n">
+        <f aca="false">AVERAGE(D3:D12)</f>
+        <v>0.1170404</v>
+      </c>
+      <c r="E13" s="20" t="n">
+        <f aca="false">AVERAGE(E3:E12)</f>
+        <v>1</v>
+      </c>
+      <c r="F13" s="20" t="n">
+        <f aca="false">AVERAGE(F3:F12)</f>
+        <v>0.1164978</v>
+      </c>
+      <c r="G13" s="20" t="n">
+        <f aca="false">AVERAGE(G3:G12)</f>
+        <v>1</v>
+      </c>
+      <c r="H13" s="20" t="n">
+        <f aca="false">AVERAGE(H3:H12)</f>
+        <v>0.2495558</v>
+      </c>
+      <c r="I13" s="20" t="n">
+        <f aca="false">AVERAGE(I3:I12)</f>
+        <v>1</v>
+      </c>
+      <c r="J13" s="20" t="n">
+        <f aca="false">AVERAGE(J3:J12)</f>
+        <v>1.8090013</v>
+      </c>
+      <c r="K13" s="20" t="n">
+        <f aca="false">AVERAGE(K3:K12)</f>
+        <v>1</v>
+      </c>
+      <c r="L13" s="20" t="n">
+        <f aca="false">AVERAGE(L3:L12)</f>
+        <v>5.35660742857143</v>
+      </c>
+      <c r="M13" s="20" t="n">
+        <f aca="false">AVERAGE(M3:M12)</f>
+        <v>0.7</v>
+      </c>
+      <c r="N13" s="20" t="n">
+        <f aca="false">AVERAGE(N3:N12)</f>
+        <v>516.2</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="N1:P1"/>
+  <mergeCells count="1">
+    <mergeCell ref="B1:M1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Added new rcm error diagrams, rcm error distribution and manipulability plots. Added standard deviation in all measurements tables
</commit_message>
<xml_diff>
--- a/data/Thesis Experiments.xlsx
+++ b/data/Thesis Experiments.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="robot_planner1" sheetId="1" state="visible" r:id="rId2"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="68">
   <si>
     <t xml:space="preserve">Robot Planner 1</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t xml:space="preserve">Average</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STD</t>
   </si>
   <si>
     <t xml:space="preserve">RRT* (max 5 seconds planning time)</t>
@@ -258,7 +261,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="#,##0.000000"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -300,12 +303,6 @@
       <name val="Cambria"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <b val="true"/>
@@ -516,7 +513,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -548,7 +545,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -624,7 +621,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -707,11 +704,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="2865916"/>
-        <c:axId val="40166364"/>
+        <c:axId val="25773412"/>
+        <c:axId val="9443091"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2865916"/>
+        <c:axId val="25773412"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -739,12 +736,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="40166364"/>
+        <c:crossAx val="9443091"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="40166364"/>
+        <c:axId val="9443091"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -781,7 +778,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2865916"/>
+        <c:crossAx val="25773412"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -840,9 +837,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>97920</xdr:colOff>
+      <xdr:colOff>97560</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>152640</xdr:rowOff>
+      <xdr:rowOff>152280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -851,7 +848,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="10197000" y="9605520"/>
-        <a:ext cx="5756040" cy="3235680"/>
+        <a:ext cx="5755680" cy="3235320"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -871,8 +868,8 @@
   </sheetPr>
   <dimension ref="A2:Q34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D4" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O33" activeCellId="0" sqref="O33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1416,14 +1413,66 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <f aca="false">STDEV(B4:B14)</f>
+        <v>0.0482302145598586</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <f aca="false">STDEV(C4:C14)</f>
+        <v>0</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <f aca="false">STDEV(D4:D14)</f>
+        <v>0.125796103456387</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <f aca="false">STDEV(E4:E14)</f>
+        <v>0</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <f aca="false">STDEV(G4:G14)</f>
+        <v>0.110001134198698</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <f aca="false">STDEV(H4:H14)</f>
+        <v>0</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <f aca="false">STDEV(I4:I14)</f>
+        <v>1.11058200783041</v>
+      </c>
+      <c r="J15" s="0" t="n">
+        <f aca="false">STDEV(J4:J14)</f>
+        <v>0.3</v>
+      </c>
+      <c r="L15" s="0" t="n">
+        <f aca="false">STDEV(L4:L14)</f>
+        <v>1.62891048879627</v>
+      </c>
+      <c r="M15" s="0" t="n">
+        <f aca="false">STDEV(M4:M14)</f>
+        <v>0.489897948556636</v>
+      </c>
+      <c r="N15" s="0" t="n">
+        <f aca="false">STDEV(N4:N14)</f>
+        <v>1.20468205991228</v>
+      </c>
+      <c r="O15" s="0" t="n">
+        <f aca="false">STDEV(O4:O14)</f>
+        <v>0.489897948556636</v>
+      </c>
+    </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -1890,7 +1939,7 @@
         <v>0</v>
       </c>
       <c r="Q28" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1944,6 +1993,59 @@
       <c r="O29" s="0" t="n">
         <f aca="false">AVERAGE(O19:O28)</f>
         <v>0.3</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <f aca="false">STDEV(B19:B29)</f>
+        <v>0.094669407516684</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <f aca="false">STDEV(C19:C29)</f>
+        <v>0</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <f aca="false">STDEV(D19:D29)</f>
+        <v>0.1046546886652</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <f aca="false">STDEV(E19:E29)</f>
+        <v>0</v>
+      </c>
+      <c r="G30" s="0" t="n">
+        <f aca="false">STDEV(G19:G29)</f>
+        <v>0.0662526939277944</v>
+      </c>
+      <c r="H30" s="0" t="n">
+        <f aca="false">STDEV(H19:H29)</f>
+        <v>0.3</v>
+      </c>
+      <c r="I30" s="0" t="n">
+        <f aca="false">STDEV(I19:I29)</f>
+        <v>0.0413376343437657</v>
+      </c>
+      <c r="J30" s="0" t="n">
+        <f aca="false">STDEV(J19:J29)</f>
+        <v>0.489897948556636</v>
+      </c>
+      <c r="L30" s="0" t="n">
+        <f aca="false">STDEV(L19:L29)</f>
+        <v>0</v>
+      </c>
+      <c r="M30" s="0" t="n">
+        <f aca="false">STDEV(M19:M29)</f>
+        <v>0.4</v>
+      </c>
+      <c r="N30" s="0" t="n">
+        <f aca="false">STDEV(N19:N29)</f>
+        <v>0.154586234275565</v>
+      </c>
+      <c r="O30" s="0" t="n">
+        <f aca="false">STDEV(O19:O29)</f>
+        <v>0.458257569495584</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1983,7 +2085,7 @@
   </sheetPr>
   <dimension ref="A1:T40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="AA25" activeCellId="0" sqref="AA25"/>
     </sheetView>
   </sheetViews>
@@ -1996,7 +2098,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -2007,7 +2109,7 @@
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="L1" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
@@ -2020,28 +2122,28 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C2" s="22"/>
       <c r="D2" s="22"/>
       <c r="E2" s="22"/>
       <c r="G2" s="22" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H2" s="22"/>
       <c r="I2" s="22"/>
       <c r="J2" s="22"/>
       <c r="L2" s="22" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M2" s="22"/>
       <c r="N2" s="22"/>
       <c r="O2" s="22"/>
       <c r="Q2" s="22" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="R2" s="22"/>
       <c r="S2" s="22"/>
@@ -2052,52 +2154,52 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D3" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>49</v>
-      </c>
       <c r="I3" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="M3" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="J3" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>49</v>
-      </c>
       <c r="N3" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="R3" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="O3" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="R3" s="8" t="s">
-        <v>49</v>
-      </c>
       <c r="S3" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="T3" s="8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2108,7 +2210,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D4" s="25" t="n">
         <v>0.065173</v>
@@ -2553,7 +2655,7 @@
         <v>1</v>
       </c>
       <c r="K12" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="L12" s="0" t="n">
         <v>1</v>
@@ -2618,7 +2720,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>1</v>
@@ -2654,41 +2756,41 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D17" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="N17" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D18" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="N18" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D19" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D20" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="N20" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D21" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -2701,13 +2803,13 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="22" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C30" s="22"/>
       <c r="D30" s="22"/>
       <c r="E30" s="22"/>
       <c r="G30" s="22" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H30" s="22"/>
       <c r="I30" s="22"/>
@@ -2718,31 +2820,31 @@
         <v>2</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D31" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H31" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="E31" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="H31" s="8" t="s">
-        <v>49</v>
-      </c>
       <c r="I31" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J31" s="8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="N31" s="26" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2774,7 +2876,7 @@
         <v>1</v>
       </c>
       <c r="N32" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2835,7 +2937,7 @@
         <v>1</v>
       </c>
       <c r="N34" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2867,7 +2969,7 @@
         <v>1</v>
       </c>
       <c r="N35" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2899,7 +3001,7 @@
         <v>1</v>
       </c>
       <c r="N36" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2962,7 +3064,7 @@
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="23" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>1</v>
@@ -3026,10 +3128,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T35"/>
+  <dimension ref="A1:T36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T9" activeCellId="0" sqref="T9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P46" activeCellId="0" sqref="P46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3041,7 +3143,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -3070,49 +3172,49 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>4</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>4</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>4</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M2" s="4" t="s">
         <v>4</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O2" s="4" t="s">
         <v>4</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="R2" s="4" t="s">
         <v>4</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="T2" s="4" t="s">
         <v>4</v>
@@ -3717,24 +3819,93 @@
         <v>0.237</v>
       </c>
     </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <f aca="false">STDEV(B3:B12)</f>
+        <v>0.0103477008981598</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <f aca="false">STDEV(C3:C12)</f>
+        <v>0</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <f aca="false">STDEV(D3:D12)</f>
+        <v>1.3355263814053</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <f aca="false">STDEV(E3:E12)</f>
+        <v>0.316227766016838</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <f aca="false">STDEV(G3:G12)</f>
+        <v>2.03859452145256</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <f aca="false">STDEV(H3:H12)</f>
+        <v>0</v>
+      </c>
+      <c r="I14" s="0" t="n">
+        <f aca="false">STDEV(I3:I12)</f>
+        <v>0.0860078221228873</v>
+      </c>
+      <c r="J14" s="0" t="n">
+        <f aca="false">STDEV(J3:J12)</f>
+        <v>0</v>
+      </c>
+      <c r="L14" s="0" t="n">
+        <f aca="false">STDEV(L3:L12)</f>
+        <v>2.12001827274405</v>
+      </c>
+      <c r="M14" s="0" t="n">
+        <f aca="false">STDEV(M3:M12)</f>
+        <v>0</v>
+      </c>
+      <c r="N14" s="0" t="n">
+        <f aca="false">STDEV(N3:N12)</f>
+        <v>2.12810285063306</v>
+      </c>
+      <c r="O14" s="0" t="n">
+        <f aca="false">STDEV(O3:O12)</f>
+        <v>0</v>
+      </c>
+      <c r="Q14" s="0" t="n">
+        <f aca="false">STDEV(Q3:Q12)</f>
+        <v>0.0883847480344381</v>
+      </c>
+      <c r="R14" s="0" t="n">
+        <f aca="false">STDEV(R3:R12)</f>
+        <v>0.168654808542314</v>
+      </c>
+      <c r="S14" s="0" t="n">
+        <f aca="false">STDEV(S3:S12)</f>
+        <v>0.314852215259089</v>
+      </c>
+      <c r="T14" s="0" t="n">
+        <f aca="false">STDEV(T3:T12)</f>
+        <v>0.418357901005029</v>
+      </c>
+    </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="O15" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="O16" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="O17" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>1</v>
@@ -3763,49 +3934,49 @@
         <v>2</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>4</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H24" s="4" t="s">
         <v>4</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J24" s="4" t="s">
         <v>4</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M24" s="4" t="s">
         <v>4</v>
       </c>
       <c r="N24" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O24" s="4" t="s">
         <v>4</v>
       </c>
       <c r="Q24" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="R24" s="4" t="s">
         <v>4</v>
       </c>
       <c r="S24" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="T24" s="4" t="s">
         <v>4</v>
@@ -4418,6 +4589,75 @@
       <c r="T35" s="0" t="n">
         <f aca="false">AVERAGE(T25:T34)</f>
         <v>0.8</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <f aca="false">STDEV(B25:B34)</f>
+        <v>0.0645550512412984</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <f aca="false">STDEV(C25:C34)</f>
+        <v>0</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <f aca="false">STDEV(D25:D34)</f>
+        <v>2.13117473375859</v>
+      </c>
+      <c r="E36" s="0" t="n">
+        <f aca="false">STDEV(E25:E34)</f>
+        <v>0</v>
+      </c>
+      <c r="G36" s="0" t="n">
+        <f aca="false">STDEV(G25:G34)</f>
+        <v>2.06929685816442</v>
+      </c>
+      <c r="H36" s="0" t="n">
+        <f aca="false">STDEV(H25:H34)</f>
+        <v>0</v>
+      </c>
+      <c r="I36" s="0" t="n">
+        <f aca="false">STDEV(I25:I34)</f>
+        <v>0.0792293809734327</v>
+      </c>
+      <c r="J36" s="0" t="n">
+        <f aca="false">STDEV(J25:J34)</f>
+        <v>0</v>
+      </c>
+      <c r="L36" s="0" t="n">
+        <f aca="false">STDEV(L25:L34)</f>
+        <v>2.31108057138398</v>
+      </c>
+      <c r="M36" s="0" t="n">
+        <f aca="false">STDEV(M25:M34)</f>
+        <v>0</v>
+      </c>
+      <c r="N36" s="0" t="n">
+        <f aca="false">STDEV(N25:N34)</f>
+        <v>2.51121605117605</v>
+      </c>
+      <c r="O36" s="0" t="n">
+        <f aca="false">STDEV(O25:O34)</f>
+        <v>0</v>
+      </c>
+      <c r="Q36" s="0" t="n">
+        <f aca="false">STDEV(Q25:Q34)</f>
+        <v>0.107534228515596</v>
+      </c>
+      <c r="R36" s="0" t="n">
+        <f aca="false">STDEV(R25:R34)</f>
+        <v>0</v>
+      </c>
+      <c r="S36" s="0" t="n">
+        <f aca="false">STDEV(S25:S34)</f>
+        <v>2.20295132090164</v>
+      </c>
+      <c r="T36" s="0" t="n">
+        <f aca="false">STDEV(T25:T34)</f>
+        <v>0.421637021355784</v>
       </c>
     </row>
   </sheetData>
@@ -4442,7 +4682,7 @@
   </sheetPr>
   <dimension ref="A1:P8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
     </sheetView>
   </sheetViews>
@@ -4454,25 +4694,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
       <c r="F1" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="J1" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
       <c r="N1" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
@@ -4482,40 +4722,40 @@
         <v>2</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="G2" s="7" t="s">
+      <c r="H2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="K2" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="K2" s="7" t="s">
+      <c r="L2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="N2" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="O2" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="N2" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>33</v>
-      </c>
       <c r="P2" s="8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4570,10 +4810,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P13"/>
+  <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O27" activeCellId="0" sqref="O27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4587,20 +4827,20 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="6.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="6.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="23.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="23.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="6.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="6.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="0" width="23.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="0" width="23.07"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="16" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -4622,43 +4862,43 @@
         <v>2</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I2" s="13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J2" s="11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="L2" s="11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="M2" s="13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N2" s="14" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="P2" s="15"/>
     </row>
@@ -4706,7 +4946,7 @@
         <v>684</v>
       </c>
       <c r="P3" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4753,7 +4993,7 @@
         <v>584</v>
       </c>
       <c r="P4" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4800,7 +5040,7 @@
         <v>339</v>
       </c>
       <c r="P5" s="18" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4847,7 +5087,7 @@
         <v>341</v>
       </c>
       <c r="P6" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5169,6 +5409,63 @@
       <c r="N13" s="20" t="n">
         <f aca="false">AVERAGE(N3:N12)</f>
         <v>516.2</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <f aca="false">STDEV(B3:B12)</f>
+        <v>0.0490021776822214</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <f aca="false">STDEV(C3:C12)</f>
+        <v>0</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <f aca="false">STDEV(D3:D12)</f>
+        <v>0.0842376736940057</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <f aca="false">STDEV(E3:E12)</f>
+        <v>0</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <f aca="false">STDEV(F3:F12)</f>
+        <v>0.0880781443842783</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <f aca="false">STDEV(G3:G12)</f>
+        <v>0</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <f aca="false">STDEV(H3:H12)</f>
+        <v>0.0789412282225764</v>
+      </c>
+      <c r="I14" s="0" t="n">
+        <f aca="false">STDEV(I3:I12)</f>
+        <v>0</v>
+      </c>
+      <c r="J14" s="0" t="n">
+        <f aca="false">STDEV(J3:J12)</f>
+        <v>2.42144847148148</v>
+      </c>
+      <c r="K14" s="0" t="n">
+        <f aca="false">STDEV(K3:K12)</f>
+        <v>0</v>
+      </c>
+      <c r="L14" s="0" t="n">
+        <f aca="false">STDEV(L3:L12)</f>
+        <v>0.0868177433647775</v>
+      </c>
+      <c r="M14" s="0" t="n">
+        <f aca="false">STDEV(M3:M12)</f>
+        <v>0.483045891539648</v>
+      </c>
+      <c r="N14" s="0" t="n">
+        <f aca="false">STDEV(N3:N12)</f>
+        <v>156.612614789202</v>
       </c>
     </row>
   </sheetData>
@@ -5192,7 +5489,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -5218,7 +5515,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -5244,7 +5541,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -5270,7 +5567,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -5296,7 +5593,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>

</xml_diff>